<commit_message>
Modificando Readme y complete el Excel.
</commit_message>
<xml_diff>
--- a/Pruebas Proyecto Python CH.xlsx
+++ b/Pruebas Proyecto Python CH.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Downloads\ProyectoFinal-main\ProyectoFinal-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1133740-F88A-4737-A04A-5A7860959A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA151438-0D3A-4CC1-B1DC-7E2C2D8C413C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{BCD56C2B-7EFC-4439-B006-08DEE2259B23}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t>Nombre del Proyecto</t>
   </si>
@@ -87,36 +87,6 @@
     <t>Todos van a una página o sección distinta</t>
   </si>
   <si>
-    <t>Edición de Instrumento</t>
-  </si>
-  <si>
-    <t>Eliminación de Instrumento Musical</t>
-  </si>
-  <si>
-    <t>Edición de Perfil de Usuario</t>
-  </si>
-  <si>
-    <t>Independientemente de la página que el usuario se encuentre, al hacer click en perfil, el usuario será dirigo a editar su perfil en el cual podrá cambiar los datos a excepción del password, el cual hay un vinculo que lo lleva a una página para el cambio de dicho password, tanto al hacer click en guardar en editar perfil como cambiar la contraseña, en ambos casos el usuario será redigido a lá página de inicio</t>
-  </si>
-  <si>
-    <t>Logout</t>
-  </si>
-  <si>
-    <t>Al hacer click en logout, el usuario automaticamente estará fuera de su sesión</t>
-  </si>
-  <si>
-    <t>Login Requerido</t>
-  </si>
-  <si>
-    <t>Cuando el usuario no esté autenticado, este será solicitado que inicie sesión para visitar las distintas páginas. La única sección que no es requerido el inicio de sesión es la sección "Conóceme"</t>
-  </si>
-  <si>
-    <t>Cuando se edita (icono de lápiz en al lado de la imagen del instrumento) la información de un instrumento musical (ejemplo bajo) el usuario es dirigido al detalle del instrumento, una vez que guarda los cambios, el usuario es redirigido a la lista de instrumentos musicales que se encontraba anteriormente (ejemplo: lista de bajos)</t>
-  </si>
-  <si>
-    <t>Dentro del listado de instrumentos(ejemplo teclados) cuando el usuario hace click en el icono de basura al lado de la imagen del instrumento, el usuario será digido a una página de eliminación del instrumento, al hacer click en eliminar, dicho instrumento será removido de la base de datos y el usuario sera redirigido a la página del listado que se encontraba anteriormente (ejemplo teclados)</t>
-  </si>
-  <si>
     <t>Contenido Marcial</t>
   </si>
   <si>
@@ -147,22 +117,46 @@
     <t>Los link redirigen a las secciones de la misma pagina.</t>
   </si>
   <si>
-    <t>Carga de Eventos</t>
-  </si>
-  <si>
-    <t>Se pueden agregar Eventos en Cartelera o en Olimpicos- mundiales.</t>
-  </si>
-  <si>
-    <t>Las imágenes de los eventos se muestran en formato de galeria.</t>
-  </si>
-  <si>
-    <t>Eliminar Eventos</t>
-  </si>
-  <si>
-    <t>Se puede aliminar un evento.</t>
-  </si>
-  <si>
-    <t>Desde la vista del editor, hay un boton en cada evento que permite eliminarlo.</t>
+    <t>Se pueden modificar y/o actualizar los Comentarios</t>
+  </si>
+  <si>
+    <t>Si el usuario esta logueado ve los botones para interactuar, sino directamente lee los comentarios</t>
+  </si>
+  <si>
+    <t>Se puede crear nuevos eventos con titulo y una imagen. Tambien se pueden editar eventos existentes o directamente eliminarlos</t>
+  </si>
+  <si>
+    <t>CRUD de Comentarios</t>
+  </si>
+  <si>
+    <t>CRUD de Eventos</t>
+  </si>
+  <si>
+    <t>Desde la vista del editor, hay un boton en cada evento que permite eliminarlo, editarlo. La visualizacion es en formato de Galería</t>
+  </si>
+  <si>
+    <t>CRUD de Indumentaria</t>
+  </si>
+  <si>
+    <t>Se pueden crear nuevas cards de indumentaria con titulo, descripción y una imagen. Tambien se pueden editar cards de indumentaria existentes o directamente eliminarlas.</t>
+  </si>
+  <si>
+    <t>El usuario logueado ve en cada Cards los botones para interactuar y el visitante solo ve una Galeria de cards</t>
+  </si>
+  <si>
+    <t>Cerrar Sesión / Logout</t>
+  </si>
+  <si>
+    <t>Se puede cerrar sesión y se redirige a la pagina principal.</t>
+  </si>
+  <si>
+    <t>Avatar</t>
+  </si>
+  <si>
+    <t>Se puede Editar y Actualizar el Avatar.</t>
+  </si>
+  <si>
+    <t>En la seccion de Editar, una vez logueado se puede agregar un Avatar o modificar uno existente</t>
   </si>
 </sst>
 </file>
@@ -550,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{524B7CD3-7E22-4FB7-BD6C-740AE7574A93}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -571,7 +565,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="1" t="s">
@@ -594,7 +588,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="F2" s="6"/>
     </row>
@@ -603,14 +597,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="F3" s="6"/>
     </row>
@@ -619,7 +613,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="1" t="s">
@@ -650,16 +644,16 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="138" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>1</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>14</v>
@@ -668,55 +662,55 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>2</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>3</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>4</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>42</v>
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>15</v>
@@ -728,107 +722,103 @@
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>6</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="180" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>7</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
-        <v>21</v>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>8</v>
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="3" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
-        <v>9</v>
-      </c>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E15" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>10</v>
-      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="3"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>